<commit_message>
More changes for colour list
</commit_message>
<xml_diff>
--- a/Source/BIT LIST.xlsx
+++ b/Source/BIT LIST.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2700" windowWidth="21570" windowHeight="7665"/>
+    <workbookView xWindow="0" yWindow="3150" windowWidth="21570" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="190">
   <si>
     <t>Bit</t>
   </si>
@@ -317,7 +317,283 @@
     <t>Galvaneal</t>
   </si>
   <si>
-    <t>=</t>
+    <t>ST36</t>
+  </si>
+  <si>
+    <t>ST30</t>
+  </si>
+  <si>
+    <t>VS29</t>
+  </si>
+  <si>
+    <t>VS26</t>
+  </si>
+  <si>
+    <t>VS24</t>
+  </si>
+  <si>
+    <t>DS29</t>
+  </si>
+  <si>
+    <t>DS26</t>
+  </si>
+  <si>
+    <t>DS24</t>
+  </si>
+  <si>
+    <t>TLF22</t>
+  </si>
+  <si>
+    <t>TLF20</t>
+  </si>
+  <si>
+    <t>TLS24</t>
+  </si>
+  <si>
+    <t>LS26</t>
+  </si>
+  <si>
+    <t>LS24</t>
+  </si>
+  <si>
+    <t>features</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>SSG</t>
+  </si>
+  <si>
+    <t>SSRP</t>
+  </si>
+  <si>
+    <t>SSRG</t>
+  </si>
+  <si>
+    <t>SSA1P</t>
+  </si>
+  <si>
+    <t>SSA1G</t>
+  </si>
+  <si>
+    <t>SSA01PU</t>
+  </si>
+  <si>
+    <t>SSA01RG</t>
+  </si>
+  <si>
+    <t>SSA01RP</t>
+  </si>
+  <si>
+    <t>SSA02G</t>
+  </si>
+  <si>
+    <t>SSA02P</t>
+  </si>
+  <si>
+    <t>SSA02RP</t>
+  </si>
+  <si>
+    <t>SSA02RG</t>
+  </si>
+  <si>
+    <t>SSB</t>
+  </si>
+  <si>
+    <t>SSBU</t>
+  </si>
+  <si>
+    <t>SSPU</t>
+  </si>
+  <si>
+    <t>SSPW</t>
+  </si>
+  <si>
+    <t>SSRPW</t>
+  </si>
+  <si>
+    <t>WFB</t>
+  </si>
+  <si>
+    <t>NFB</t>
+  </si>
+  <si>
+    <t>WFG</t>
+  </si>
+  <si>
+    <t>NFG</t>
+  </si>
+  <si>
+    <t>WFP</t>
+  </si>
+  <si>
+    <t>NFP</t>
+  </si>
+  <si>
+    <t>WFPU</t>
+  </si>
+  <si>
+    <t>NFPU</t>
+  </si>
+  <si>
+    <t>WFPW</t>
+  </si>
+  <si>
+    <t>NFPW</t>
+  </si>
+  <si>
+    <t>WFRG</t>
+  </si>
+  <si>
+    <t>NFRG</t>
+  </si>
+  <si>
+    <t>WFRP</t>
+  </si>
+  <si>
+    <t>NFRP</t>
+  </si>
+  <si>
+    <t>WFRPW</t>
+  </si>
+  <si>
+    <t>NFRPW</t>
+  </si>
+  <si>
+    <t>WPA01G</t>
+  </si>
+  <si>
+    <t>NPA01G</t>
+  </si>
+  <si>
+    <t>WPA01P</t>
+  </si>
+  <si>
+    <t>NPA01P</t>
+  </si>
+  <si>
+    <t>WPA01RG</t>
+  </si>
+  <si>
+    <t>NPA01RG</t>
+  </si>
+  <si>
+    <t>WPA01RP</t>
+  </si>
+  <si>
+    <t>NPA01RP</t>
+  </si>
+  <si>
+    <t>WPA02G</t>
+  </si>
+  <si>
+    <t>NPA02G</t>
+  </si>
+  <si>
+    <t>WPA02P</t>
+  </si>
+  <si>
+    <t>NPA02P</t>
+  </si>
+  <si>
+    <t>WPA02RG</t>
+  </si>
+  <si>
+    <t>NPA02RG</t>
+  </si>
+  <si>
+    <t>WPA02RP</t>
+  </si>
+  <si>
+    <t>NPA02RP</t>
+  </si>
+  <si>
+    <t>WPB</t>
+  </si>
+  <si>
+    <t>NPB</t>
+  </si>
+  <si>
+    <t>WPG</t>
+  </si>
+  <si>
+    <t>NPG</t>
+  </si>
+  <si>
+    <t>WPP</t>
+  </si>
+  <si>
+    <t>NPP</t>
+  </si>
+  <si>
+    <t>WPPU</t>
+  </si>
+  <si>
+    <t>NPPU</t>
+  </si>
+  <si>
+    <t>WPPW</t>
+  </si>
+  <si>
+    <t>NPPW</t>
+  </si>
+  <si>
+    <t>WPRG</t>
+  </si>
+  <si>
+    <t>NPRG</t>
+  </si>
+  <si>
+    <t>WPRP</t>
+  </si>
+  <si>
+    <t>NPRP</t>
+  </si>
+  <si>
+    <t>WPRPU</t>
+  </si>
+  <si>
+    <t>NPRPU</t>
+  </si>
+  <si>
+    <t>WPRPW</t>
+  </si>
+  <si>
+    <t>NPRPW</t>
+  </si>
+  <si>
+    <t>DSG</t>
+  </si>
+  <si>
+    <t>DSP</t>
+  </si>
+  <si>
+    <t>DSPU</t>
+  </si>
+  <si>
+    <t>DSPW</t>
+  </si>
+  <si>
+    <t>DSRG</t>
+  </si>
+  <si>
+    <t>DSRP</t>
+  </si>
+  <si>
+    <t>DSRPW</t>
+  </si>
+  <si>
+    <t>VSG</t>
+  </si>
+  <si>
+    <t>VSP</t>
+  </si>
+  <si>
+    <t>VSPU</t>
+  </si>
+  <si>
+    <t>VSPW</t>
   </si>
 </sst>
 </file>
@@ -333,7 +609,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,6 +646,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -383,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -393,6 +699,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,25 +987,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:AA55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="17.7109375" style="2" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="18.85546875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="8" width="14.28515625" style="2" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="2"/>
+    <col min="12" max="12" width="18.85546875" style="2" customWidth="1"/>
+    <col min="13" max="16" width="9.140625" style="2"/>
+    <col min="17" max="17" width="13" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -704,8 +1022,55 @@
       <c r="E1" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -718,33 +1083,52 @@
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4">
-        <f>B20+B26+B27+B32+B33</f>
-        <v>1777664</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="9">
+        <f>B20+B26+B27+B32+B33+B35+B36+B37+B38+B39</f>
+        <v>131801088</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="13">
+        <f>B2+B32+B20</f>
+        <v>532481</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="L2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="2">
+      <c r="M2" s="10">
         <f>$B$2</f>
         <v>1</v>
       </c>
-      <c r="K2" s="2">
+      <c r="N2" s="10"/>
+      <c r="O2" s="10">
         <f>$B$3+$B$18</f>
         <v>2050</v>
       </c>
-      <c r="L2" s="2">
+      <c r="P2" s="10">
         <f>$B$5+$B$28</f>
         <v>262152</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10">
+        <f>$B$4+$B$28</f>
+        <v>262148</v>
+      </c>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f>SUM(B2:B14)</f>
         <v>255</v>
@@ -759,31 +1143,54 @@
       <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="4">
-        <f>B18+B20+B26+B27+B32+B33</f>
-        <v>1779712</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="E3" s="9">
+        <f>B18+B20+B26+B27+B32+B33+B34+B35+B36+B37+B38+B39</f>
+        <v>133900288</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="14">
+        <f>B2+B43+B33+B20</f>
+        <v>1074798593</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="L3" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="2">
-        <f t="shared" ref="I3:I19" si="0">$B$2</f>
+      <c r="M3" s="10">
+        <f t="shared" ref="M3:M19" si="0">$B$2</f>
         <v>1</v>
       </c>
-      <c r="J3" s="2">
+      <c r="N3" s="10">
         <f>$B$3+$B$20</f>
         <v>8194</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10">
+        <f t="shared" ref="S3:S16" si="1">$B$4+$B$28</f>
+        <v>262148</v>
+      </c>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="4">
-        <f t="shared" ref="B4:B43" si="1">B3*2</f>
+        <f t="shared" ref="B4:B43" si="2">B3*2</f>
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -792,36 +1199,58 @@
       <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4">
-        <f>B20+B26+B27+B28+B32+B33</f>
-        <v>2039808</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="E4" s="9">
+        <f>B20+B26+B27+B28+B32+B33+B38+B39</f>
+        <v>102703104</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="13">
+        <f>B2+B33+B20</f>
+        <v>1056769</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="L4" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="2">
+      <c r="M4" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J4" s="2">
-        <f t="shared" ref="J4:J5" si="2">$B$3+$B$20</f>
+      <c r="N4" s="10">
+        <f t="shared" ref="N4:N5" si="3">$B$3+$B$20</f>
         <v>8194</v>
       </c>
-      <c r="L4" s="2">
+      <c r="O4" s="10"/>
+      <c r="P4" s="10">
         <f>$B$5+$B$28</f>
         <v>262152</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10">
+        <f t="shared" si="1"/>
+        <v>262148</v>
+      </c>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f>B2+B3+B4+B7+B5</f>
         <v>47</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -830,35 +1259,57 @@
       <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="4">
-        <f>B20+B26+B27+B28+B32</f>
-        <v>991232</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="E5" s="9">
+        <f>B20+B26+B27+B28+B32+B38+B39</f>
+        <v>101654528</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H5" s="14">
+        <f>B2+B33+B43+B20</f>
+        <v>1074798593</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="L5" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="I5" s="2">
+      <c r="M5" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J5" s="2">
-        <f t="shared" si="2"/>
+      <c r="N5" s="10">
+        <f t="shared" si="3"/>
         <v>8194</v>
       </c>
-      <c r="L5" s="2">
-        <f t="shared" ref="L5:L16" si="3">$B$5+$B$28</f>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10">
+        <f t="shared" ref="P5:P16" si="4">$B$5+$B$28</f>
         <v>262152</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10">
+        <f t="shared" si="1"/>
+        <v>262148</v>
+      </c>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -871,32 +1322,57 @@
         <f>B16+B17+B25+B26</f>
         <v>99840</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6" s="13">
+        <f>B2+B35+B32+B20</f>
+        <v>4726785</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="L6" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="I6" s="2">
+      <c r="M6" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K6" s="2">
-        <f t="shared" ref="K6:K7" si="4">$B$3+$B$18</f>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10">
+        <f t="shared" ref="O6:O7" si="5">$B$3+$B$18</f>
         <v>2050</v>
       </c>
-      <c r="L6" s="2">
-        <f t="shared" si="3"/>
+      <c r="P6" s="10">
+        <f t="shared" si="4"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10">
+        <f t="shared" si="1"/>
+        <v>262148</v>
+      </c>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10">
+        <f>$B$7+$B$24</f>
+        <v>16416</v>
+      </c>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <f>B2+B3+B4+B5+B6+B9</f>
         <v>159</v>
       </c>
       <c r="B7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -909,31 +1385,53 @@
         <f>B15+B24+B25+B26</f>
         <v>114944</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7" s="14">
+        <f>B2+B35+B43+B32+B20</f>
+        <v>1078468609</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="L7" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="I7" s="2">
+      <c r="M7" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K7" s="2">
+      <c r="N7" s="10"/>
+      <c r="O7" s="10">
+        <f t="shared" si="5"/>
+        <v>2050</v>
+      </c>
+      <c r="P7" s="10">
         <f t="shared" si="4"/>
-        <v>2050</v>
-      </c>
-      <c r="L7" s="2">
-        <f t="shared" si="3"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10">
+        <f t="shared" si="1"/>
+        <v>262148</v>
+      </c>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -946,32 +1444,66 @@
         <f>B19+B25+B26+B27</f>
         <v>233472</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8" s="14">
+        <f>B2+B35+B39+B32+B20</f>
+        <v>71835649</v>
+      </c>
+      <c r="K8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="L8" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="I8" s="2">
+      <c r="M8" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J8" s="2">
-        <f t="shared" ref="J8" si="5">$B$3+$B$20</f>
+      <c r="N8" s="10">
+        <f t="shared" ref="N8" si="6">$B$3+$B$20</f>
         <v>8194</v>
       </c>
-      <c r="L8" s="2">
-        <f t="shared" si="3"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10">
+        <f t="shared" si="4"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q8" s="10">
+        <f>$B$5+$B$27</f>
+        <v>131080</v>
+      </c>
+      <c r="R8" s="10">
+        <f>$B$5+$B$26</f>
+        <v>65544</v>
+      </c>
+      <c r="S8" s="10">
+        <f t="shared" si="1"/>
+        <v>262148</v>
+      </c>
+      <c r="T8" s="10">
+        <f>$B$4+$B$27</f>
+        <v>131076</v>
+      </c>
+      <c r="U8" s="10">
+        <f>$B$4+$B$26</f>
+        <v>65540</v>
+      </c>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <f>B2+B4+B5+B8</f>
         <v>77</v>
       </c>
       <c r="B9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>128</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -984,18 +1516,42 @@
         <f>B18+B20+B24+B25+B26+B27</f>
         <v>256000</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" s="14">
+        <f>B2+B35+B33+B43+B20</f>
+        <v>1078992897</v>
+      </c>
+      <c r="K9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="L9" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="L9" s="2">
-        <f t="shared" si="3"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10">
+        <f t="shared" si="4"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10">
+        <f t="shared" si="1"/>
+        <v>262148</v>
+      </c>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="10"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
@@ -1003,26 +1559,48 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" s="13">
+        <f>B2+B35+B33+B20</f>
+        <v>5251073</v>
+      </c>
+      <c r="K10" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="L10" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="I10" s="2">
+      <c r="M10" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K10" s="2">
-        <f t="shared" ref="K10:K12" si="6">$B$3+$B$18</f>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10">
+        <f t="shared" ref="O10:O12" si="7">$B$3+$B$18</f>
         <v>2050</v>
       </c>
-      <c r="L10" s="2">
-        <f t="shared" si="3"/>
+      <c r="P10" s="10">
+        <f t="shared" si="4"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10">
+        <f t="shared" si="1"/>
+        <v>262148</v>
+      </c>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <f>B2+B4+B5+B8</f>
         <v>77</v>
@@ -1031,22 +1609,57 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" s="14">
+        <f>B2+B36+B43+B32+B20</f>
+        <v>1082662913</v>
+      </c>
+      <c r="K11" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="L11" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="I11" s="2">
+      <c r="M11" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K11" s="2">
-        <f t="shared" si="6"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10">
+        <f t="shared" si="7"/>
         <v>2050</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10">
+        <f>$B$6</f>
+        <v>16</v>
+      </c>
+      <c r="W11" s="10">
+        <f>$B$7+$B$25</f>
+        <v>32800</v>
+      </c>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10">
+        <f>$B$7+$B$26+$B$34</f>
+        <v>2162720</v>
+      </c>
+      <c r="Z11" s="10">
+        <f>$B$8+$B$27</f>
+        <v>131136</v>
+      </c>
+      <c r="AA11" s="10">
+        <f>$B$8+$B$26</f>
+        <v>65600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>34</v>
       </c>
@@ -1054,26 +1667,48 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="13">
+        <f>B2+B36+B32+B20</f>
+        <v>8921089</v>
+      </c>
+      <c r="K12" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="L12" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="2">
+      <c r="M12" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K12" s="2">
-        <f t="shared" si="6"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10">
+        <f t="shared" si="7"/>
         <v>2050</v>
       </c>
-      <c r="L12" s="2">
-        <f t="shared" si="3"/>
+      <c r="P12" s="10">
+        <f t="shared" si="4"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10">
+        <f t="shared" si="1"/>
+        <v>262148</v>
+      </c>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <f>B9</f>
         <v>128</v>
@@ -1082,39 +1717,86 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="13">
+        <f>B2+B36+B33+B20</f>
+        <v>9445377</v>
+      </c>
+      <c r="K13" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="L13" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="L13" s="2">
-        <f t="shared" si="3"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10">
+        <f t="shared" si="4"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10">
+        <f t="shared" si="1"/>
+        <v>262148</v>
+      </c>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="10"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="14">
+        <f>B2+B36+B33+B43+B20</f>
+        <v>1083187201</v>
+      </c>
+      <c r="K14" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="L14" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="I14" s="2">
+      <c r="M14" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K14" s="2">
-        <f t="shared" ref="K14:K19" si="7">$B$3+$B$18</f>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10">
+        <f t="shared" ref="O14:O19" si="8">$B$3+$B$18</f>
         <v>2050</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10">
+        <f t="shared" si="1"/>
+        <v>262148</v>
+      </c>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1130,32 +1812,54 @@
         <f>B7+B15+B24+B25+B26</f>
         <v>114976</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="H15" s="13">
+        <f>B2+B37+B32+B20</f>
+        <v>17309697</v>
+      </c>
+      <c r="K15" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="L15" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="2">
+      <c r="M15" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K15" s="2">
-        <f t="shared" si="7"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10">
+        <f t="shared" si="8"/>
         <v>2050</v>
       </c>
-      <c r="L15" s="2">
-        <f t="shared" si="3"/>
+      <c r="P15" s="10">
+        <f t="shared" si="4"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10">
+        <f t="shared" si="1"/>
+        <v>262148</v>
+      </c>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f>SUM(B15:B20)</f>
         <v>16128</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>512</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1166,29 +1870,51 @@
         <f>B6+B16+B17+B25+B26</f>
         <v>99856</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" s="14">
+        <f>B2+B37+B39+B32+B20</f>
+        <v>84418561</v>
+      </c>
+      <c r="K16" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="L16" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="I16" s="2">
+      <c r="M16" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K16" s="2">
-        <f t="shared" si="7"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10">
+        <f t="shared" si="8"/>
         <v>2050</v>
       </c>
-      <c r="L16" s="2">
-        <f t="shared" si="3"/>
+      <c r="P16" s="10">
+        <f t="shared" si="4"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10">
+        <f t="shared" si="1"/>
+        <v>262148</v>
+      </c>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1024</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1199,25 +1925,45 @@
         <f>B6+B17+B18+B25+B26</f>
         <v>101392</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="H17" s="14">
+        <f>B2+B39+B32+B20</f>
+        <v>67641345</v>
+      </c>
+      <c r="K17" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="L17" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="I17" s="2">
+      <c r="M17" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K17" s="2">
-        <f t="shared" si="7"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10">
+        <f t="shared" si="8"/>
         <v>2050</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2048</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1228,25 +1974,45 @@
         <f>B3+B9++B18+B20+B24+B25+B26+B27+B32+B33</f>
         <v>1828994</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="13">
+        <f>B2+B38+B32+B20</f>
+        <v>34086913</v>
+      </c>
+      <c r="K18" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="L18" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="I18" s="2">
+      <c r="M18" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K18" s="2">
-        <f t="shared" si="7"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10">
+        <f t="shared" si="8"/>
         <v>2050</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="10"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4096</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1257,25 +2023,45 @@
         <f>B8+B25+B26+B27+B19</f>
         <v>233536</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="13">
+        <f>B2+B33+B38+B20</f>
+        <v>34611201</v>
+      </c>
+      <c r="K19" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="L19" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="I19" s="2">
+      <c r="M19" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K19" s="2">
-        <f t="shared" si="7"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10">
+        <f t="shared" si="8"/>
         <v>2050</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8192</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1286,69 +2072,169 @@
         <f>B2+B3+B4+B5+B9+B18+B20+B24+B25+B26+B27+B28+B32+B33</f>
         <v>2091151</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J20" s="12"/>
+      <c r="K20" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="L20" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="L20" s="2">
-        <f t="shared" ref="L20:L27" si="8">$B$5+$B$28</f>
-        <v>262152</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10">
+        <f>$B$5+$B$27</f>
+        <v>131080</v>
+      </c>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10">
+        <f>$B$4+$B$27</f>
+        <v>131076</v>
+      </c>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="10"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="J21" s="12"/>
+      <c r="K21" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="L21" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="L21" s="2">
-        <f t="shared" si="8"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10">
+        <f t="shared" ref="P21:P27" si="9">$B$5+$B$28</f>
         <v>262152</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10">
+        <f t="shared" ref="S21:S27" si="10">$B$4+$B$28</f>
+        <v>262148</v>
+      </c>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="J22" s="12"/>
+      <c r="K22" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="L22" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="L22" s="2">
-        <f t="shared" si="8"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10">
+        <f t="shared" si="9"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10">
+        <f t="shared" si="10"/>
+        <v>262148</v>
+      </c>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="J23" s="12"/>
+      <c r="K23" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="L23" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="L23" s="2">
-        <f t="shared" si="8"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10">
+        <f t="shared" si="9"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10">
+        <f t="shared" si="10"/>
+        <v>262148</v>
+      </c>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -1364,24 +2250,49 @@
         <f>B7+B9+B15++B18+B20+B24+B25+B26+B27</f>
         <v>256416</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="J24" s="12"/>
+      <c r="K24" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="L24" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="L24" s="2">
-        <f t="shared" si="8"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10">
+        <f t="shared" si="9"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10">
+        <f t="shared" si="10"/>
+        <v>262148</v>
+      </c>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="10"/>
+      <c r="AA24" s="10"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <f>SUM(B24:B28)</f>
         <v>507904</v>
       </c>
       <c r="B25" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32768</v>
       </c>
       <c r="C25" s="5">
@@ -1392,21 +2303,46 @@
         <f>B7+B6+B9+B8+B15+B16+B17+B18+B19+B20+B24+B25+B26+B27</f>
         <v>262128</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="J25" s="12"/>
+      <c r="K25" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="L25" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="L25" s="2">
-        <f t="shared" si="8"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10">
+        <f t="shared" si="9"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10">
+        <f t="shared" si="10"/>
+        <v>262148</v>
+      </c>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="10"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65536</v>
       </c>
       <c r="C26" s="5">
@@ -1417,29 +2353,61 @@
         <f>B9+B7+B6+B5+B4+B3+B2+B8+B15+B16+B17+B18+B19+B20+B24+B25+B26+B27+B28+B32+B33</f>
         <v>2097151</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="J26" s="12"/>
+      <c r="K26" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="L26" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="I26" s="2">
-        <f t="shared" ref="I26" si="9">$B$2</f>
+      <c r="M26" s="10">
+        <f t="shared" ref="M26" si="11">$B$2</f>
         <v>1</v>
       </c>
-      <c r="K26" s="2">
+      <c r="N26" s="10"/>
+      <c r="O26" s="10">
         <f>$B$3+$B$18</f>
         <v>2050</v>
       </c>
-      <c r="L26" s="2">
-        <f t="shared" si="8"/>
+      <c r="P26" s="10">
+        <f t="shared" si="9"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10">
+        <f t="shared" si="10"/>
+        <v>262148</v>
+      </c>
+      <c r="T26" s="10">
+        <f>$B$4+$B$27</f>
+        <v>131076</v>
+      </c>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10">
+        <f>$B$6</f>
+        <v>16</v>
+      </c>
+      <c r="W26" s="10">
+        <f>$B$7+$B$25</f>
+        <v>32800</v>
+      </c>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="10"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>131072</v>
       </c>
       <c r="C27" s="5">
@@ -1450,21 +2418,52 @@
         <f>B2+B3+B4+B5+B8+B9+B18+B19+B24+B25+B26+B27+B28+B32+B33</f>
         <v>2087119</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="K27" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="L27" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L27" s="2">
-        <f t="shared" si="8"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10">
+        <f t="shared" si="9"/>
         <v>262152</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10">
+        <f t="shared" si="10"/>
+        <v>262148</v>
+      </c>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10">
+        <f>$B$8+$B$27</f>
+        <v>131136</v>
+      </c>
+      <c r="AA27" s="10">
+        <f>$B$8+$B$26</f>
+        <v>65600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>262144</v>
       </c>
       <c r="C28" s="5">
@@ -1475,35 +2474,82 @@
         <f>B4+B5+B26+B27+B28+B32+B33</f>
         <v>2031628</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="J28" s="12"/>
+      <c r="K28" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="L28" s="10" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
+      <c r="X28" s="10"/>
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="10"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G29" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G30" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G31" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>29</v>
       </c>
@@ -1515,12 +2561,20 @@
         <v>35</v>
       </c>
       <c r="D32" s="6"/>
-      <c r="E32" s="6">
-        <f>B2+B3+B4+B5+B18+B20+B26+B27+B28+B32+B33</f>
-        <v>2041871</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="11">
+        <f>B2+B3+B4+B5+B18+B20+B26+B27+B28+B32+B33+B34+B35+B36+B37+B38+B39</f>
+        <v>134162447</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <f>SUM(B32:B33)</f>
         <v>1572864</v>
@@ -1537,11 +2591,21 @@
         <f>B2+B3+B4+B18+B20+B26+B27+B28+B32+B33</f>
         <v>2041863</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+      <c r="G33" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="J33" s="12"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="B34" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2097152</v>
       </c>
       <c r="C34" s="7" t="s">
@@ -1549,96 +2613,264 @@
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+      <c r="G34" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="J34" s="12"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <f>SUM(B34:B39)</f>
+        <v>132120576</v>
+      </c>
       <c r="B35" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4194304</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>38</v>
       </c>
       <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="8">
+        <f>B2+B20+B27+B26+B32+B33+B43+B39</f>
+        <v>1142628353</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="J35" s="12"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8388608</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="8">
+        <f>B2+B32+B33+B43+B20+B27+B26</f>
+        <v>1075519489</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="J36" s="12"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16777216</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>40</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="7">
+        <f>B2+B20+B27+B26+B32+B38</f>
+        <v>34283521</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="J37" s="12"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33554432</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="7">
+        <f>B2+B20+B32+B35+B37+B27+B26</f>
+        <v>21700609</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="J38" s="12"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67108864</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="7">
+        <f>B2+B20+B27+B26+B32+B33</f>
+        <v>1777665</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="J39" s="12"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>134217728</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="G40" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J40" s="12"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <f t="shared" si="2"/>
+        <v>268435456</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="J41" s="12"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="3">
+        <f t="shared" si="2"/>
+        <v>536870912</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="J42" s="12"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="3">
+        <f t="shared" si="2"/>
+        <v>1073741824</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="3">
-        <f t="shared" si="1"/>
-        <v>268435456</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="3">
-        <f t="shared" si="1"/>
-        <v>536870912</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="3">
-        <f t="shared" si="1"/>
-        <v>1073741824</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G43" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="J43" s="12"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
+      <c r="G44" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="J44" s="12"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G45" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="H45" s="16"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G46" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="H46" s="16"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G47" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H47" s="16"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G48" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="H48" s="16"/>
+    </row>
+    <row r="49" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G49" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="H49" s="16"/>
+    </row>
+    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G50" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="H50" s="16"/>
+    </row>
+    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G51" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="H51" s="16"/>
+    </row>
+    <row r="52" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G52" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G53" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="54" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G54" s="15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G55" s="15" t="s">
+        <v>189</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>